<commit_message>
changing code to work with .csv files instead of .xlsx
</commit_message>
<xml_diff>
--- a/data/rrv_volatiles_pca_contribution_table_pca_dat.xlsx
+++ b/data/rrv_volatiles_pca_contribution_table_pca_dat.xlsx
@@ -1,21 +1,107 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uflorida-my.sharepoint.com/personal/afife_ufl_edu/Documents/DISSERTATION/MANUSCRIPT/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_8D61FDCE8F79A8D366075C52F3F612B7E8CDBCD9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E015D0E-98DC-4767-A6D7-48AC23A1A42E}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>Chemical</t>
+  </si>
+  <si>
+    <t>PCA1</t>
+  </si>
+  <si>
+    <t>PCA2</t>
+  </si>
+  <si>
+    <t>PCA3</t>
+  </si>
+  <si>
+    <t>Pinene &lt;1R-alpha-&gt;</t>
+  </si>
+  <si>
+    <t>Pinene &lt;alpha-&gt;</t>
+  </si>
+  <si>
+    <t>Pinene &lt;beta-&gt;</t>
+  </si>
+  <si>
+    <t>Carene, &lt;3-&gt;</t>
+  </si>
+  <si>
+    <t>Carene &lt;delta-3&gt;</t>
+  </si>
+  <si>
+    <t>Phellandrene &lt;beta-&gt;</t>
+  </si>
+  <si>
+    <t>p-Cymene</t>
+  </si>
+  <si>
+    <t>D-Limonene</t>
+  </si>
+  <si>
+    <t>Limonene oxide, trans-</t>
+  </si>
+  <si>
+    <t>Copaene &lt;alpha-&gt;</t>
+  </si>
+  <si>
+    <t>Copaene &lt;beta-&gt;</t>
+  </si>
+  <si>
+    <t>Bourbonene &lt;beta-&gt;</t>
+  </si>
+  <si>
+    <t>Bergamotene &lt;alpha-, cis-&gt;</t>
+  </si>
+  <si>
+    <t>Caryophyllene</t>
+  </si>
+  <si>
+    <t>Caryophyllene oxide</t>
+  </si>
+  <si>
+    <t>Caryophyllene &lt;9-epi-(E)-&gt;</t>
+  </si>
+  <si>
+    <t>Murrolene &lt;alpha-&gt;</t>
+  </si>
+  <si>
+    <t>Murrolene &lt;gamma-&gt;</t>
+  </si>
+  <si>
+    <t>Muurrolene &lt;gamma-&gt;</t>
+  </si>
+  <si>
+    <t>Farnesene &lt;(E,E)-, alpha-&gt;</t>
+  </si>
+  <si>
+    <t>Farnesene &lt;(E)-, beta-&gt;</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +149,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -109,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +235,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +287,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,56 +480,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Chemical</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>PCA1</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PCA2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PCA3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Pinene &lt;1R-alpha-&gt;</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>6.554688847719173e-006</v>
+        <v>6.5546888477191733E-6</v>
       </c>
       <c r="C2">
-        <v>1.483263018052667e-007</v>
+        <v>1.4832630180526671E-7</v>
       </c>
       <c r="D2">
-        <v>9.287095734755803e-008</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Pinene &lt;alpha-&gt;</t>
-        </is>
+        <v>9.2870957347558028E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
       </c>
       <c r="B3">
         <v>1.117951645461795</v>
@@ -408,311 +531,273 @@
         <v>0.3148965791958474</v>
       </c>
       <c r="D3">
-        <v>6.212334800222965</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Pinene &lt;beta-&gt;</t>
-        </is>
+        <v>6.2123348002229646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>1.327499825716408</v>
+        <v>1.3274998257164079</v>
       </c>
       <c r="C4">
-        <v>0.1799170849645376</v>
+        <v>0.17991708496453759</v>
       </c>
       <c r="D4">
-        <v>7.289603767649963</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Carene, &lt;3-&gt;</t>
-        </is>
+        <v>7.2896037676499628</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>0.0003008466283978323</v>
+        <v>3.0084662839783232E-4</v>
       </c>
       <c r="C5">
-        <v>6.069565131753935e-005</v>
+        <v>6.0695651317539352E-5</v>
       </c>
       <c r="D5">
-        <v>0.04923105356227622</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Carene &lt;delta-3&gt;</t>
-        </is>
+        <v>4.9231053562276222E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>5.180596937136926e-006</v>
+        <v>5.1805969371369256E-6</v>
       </c>
       <c r="C6">
-        <v>5.701178703222212e-006</v>
+        <v>5.7011787032222124E-6</v>
       </c>
       <c r="D6">
-        <v>0.003097342810416124</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Phellandrene &lt;beta-&gt;</t>
-        </is>
+        <v>3.0973428104161239E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>2.589029324659029e-008</v>
+        <v>2.5890293246590289E-8</v>
       </c>
       <c r="C7">
-        <v>5.046169826689923e-009</v>
+        <v>5.0461698266899227E-9</v>
       </c>
       <c r="D7">
-        <v>3.9309942968903e-006</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>p-Cymene</t>
-        </is>
+        <v>3.9309942968903E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>2.256962881330064e-006</v>
+        <v>2.2569628813300638E-6</v>
       </c>
       <c r="C8">
-        <v>3.699288318719675e-007</v>
+        <v>3.6992883187196751E-7</v>
       </c>
       <c r="D8">
-        <v>0.0001568684938616696</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>D-Limonene</t>
-        </is>
+        <v>1.5686849386166961E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
       </c>
       <c r="B9">
         <v>0.4792772862951955</v>
       </c>
       <c r="C9">
-        <v>0.04192820955004242</v>
+        <v>4.1928209550042422E-2</v>
       </c>
       <c r="D9">
-        <v>22.07833431368135</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Limonene oxide, trans-</t>
-        </is>
+        <v>22.078334313681349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>8.458219433140276e-012</v>
+        <v>8.4582194331402759E-12</v>
       </c>
       <c r="C10">
-        <v>4.768251608430652e-014</v>
+        <v>4.7682516084306518E-14</v>
       </c>
       <c r="D10">
-        <v>2.777275066491221e-011</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Copaene &lt;alpha-&gt;</t>
-        </is>
+        <v>2.777275066491221E-11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>0.01548949119504503</v>
+        <v>1.548949119504503E-2</v>
       </c>
       <c r="C11">
-        <v>0.02958728968357749</v>
+        <v>2.9587289683577489E-2</v>
       </c>
       <c r="D11">
-        <v>0.02141189154573871</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Copaene &lt;beta-&gt;</t>
-        </is>
+        <v>2.141189154573871E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>0.167566164920581</v>
+        <v>0.16756616492058099</v>
       </c>
       <c r="C12">
-        <v>0.01732383277366371</v>
+        <v>1.732383277366371E-2</v>
       </c>
       <c r="D12">
         <v>0.2195929998856731</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Bourbonene &lt;beta-&gt;</t>
-        </is>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>4.942080864867774e-006</v>
+        <v>4.9420808648677739E-6</v>
       </c>
       <c r="C13">
-        <v>4.9410441880111e-006</v>
+        <v>4.9410441880110999E-6</v>
       </c>
       <c r="D13">
-        <v>0.002715931386013186</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Bergamotene &lt;alpha-, cis-&gt;</t>
-        </is>
+        <v>2.7159313860131858E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>5.451889271412953e-010</v>
+        <v>5.4518892714129528E-10</v>
       </c>
       <c r="C14">
-        <v>4.432686277064773e-012</v>
+        <v>4.4326862770647729E-12</v>
       </c>
       <c r="D14">
-        <v>4.696326674209347e-008</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Caryophyllene</t>
-        </is>
+        <v>4.6963266742093467E-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>8.509613464039967</v>
+        <v>8.5096134640399672</v>
       </c>
       <c r="C15">
-        <v>0.9945675097876799</v>
+        <v>0.99456750978767994</v>
       </c>
       <c r="D15">
-        <v>22.33096517648155</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Caryophyllene oxide</t>
-        </is>
+        <v>22.330965176481548</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>1.608276596523557e-007</v>
+        <v>1.6082765965235571E-7</v>
       </c>
       <c r="C16">
-        <v>4.031598239397055e-008</v>
+        <v>4.0315982393970551E-8</v>
       </c>
       <c r="D16">
-        <v>1.627171312105399e-005</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Caryophyllene &lt;9-epi-(E)-&gt;</t>
-        </is>
+        <v>1.6271713121053989E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
       </c>
       <c r="B17">
         <v>0.2428848098150885</v>
       </c>
       <c r="C17">
-        <v>0.02615229131923879</v>
+        <v>2.6152291319238789E-2</v>
       </c>
       <c r="D17">
         <v>0.2810835547850381</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Murrolene &lt;alpha-&gt;</t>
-        </is>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>1.656336189657879e-005</v>
+        <v>1.6563361896578789E-5</v>
       </c>
       <c r="C18">
-        <v>1.216584652155503e-005</v>
+        <v>1.216584652155503E-5</v>
       </c>
       <c r="D18">
-        <v>0.007548016357117769</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Murrolene &lt;gamma-&gt;</t>
-        </is>
+        <v>7.5480163571177688E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>21</v>
       </c>
       <c r="B19">
-        <v>0.0250808956316093</v>
+        <v>2.5080895631609298E-2</v>
       </c>
       <c r="C19">
-        <v>0.02017504209678385</v>
+        <v>2.0175042096783849E-2</v>
       </c>
       <c r="D19">
         <v>12.22693404627686</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Muurrolene &lt;gamma-&gt;</t>
-        </is>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>79.12588461854807</v>
+        <v>79.125884618548071</v>
       </c>
       <c r="C20">
         <v>7.784478708915489</v>
       </c>
       <c r="D20">
-        <v>6.003707804064923</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Farnesene &lt;(E,E)-, alpha-&gt;</t>
-        </is>
+        <v>6.0037078040649234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
       </c>
       <c r="B21">
-        <v>8.939811133294654</v>
+        <v>8.9398111332946542</v>
       </c>
       <c r="C21">
-        <v>90.56363987265287</v>
+        <v>90.563639872652871</v>
       </c>
       <c r="D21">
-        <v>0.004397739055683266</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Farnesene &lt;(E)-, beta-&gt;</t>
-        </is>
+        <v>4.3977390556832656E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>24</v>
       </c>
       <c r="B22">
-        <v>0.0486041334901599</v>
+        <v>4.86041334901599E-2</v>
       </c>
       <c r="C22">
-        <v>0.02724951171778247</v>
+        <v>2.7249511717782469E-2</v>
       </c>
       <c r="D22">
-        <v>23.26886435117117</v>
+        <v>23.268864351171171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>